<commit_message>
TB incluyendo Ranking terminado
</commit_message>
<xml_diff>
--- a/AG/AG/testbench/resultados.xlsx
+++ b/AG/AG/testbench/resultados.xlsx
@@ -1629,24 +1629,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1658,13 +1640,7 @@
     <xf numFmtId="164" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="6" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1676,55 +1652,49 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="16" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1745,10 +1715,40 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1830,24 +1830,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="93480064"/>
-        <c:axId val="126715008"/>
+        <c:axId val="83365888"/>
+        <c:axId val="83367424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="93480064"/>
+        <c:axId val="83365888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126715008"/>
+        <c:crossAx val="83367424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="126715008"/>
+        <c:axId val="83367424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1855,7 +1855,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93480064"/>
+        <c:crossAx val="83365888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1864,7 +1864,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1932,24 +1932,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="109948288"/>
-        <c:axId val="91533696"/>
+        <c:axId val="83387520"/>
+        <c:axId val="83389056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="109948288"/>
+        <c:axId val="83387520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91533696"/>
+        <c:crossAx val="83389056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91533696"/>
+        <c:axId val="83389056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1957,7 +1957,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109948288"/>
+        <c:crossAx val="83387520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1966,7 +1966,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2002,7 +2002,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2148,13 +2147,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:marker val="1"/>
-        <c:axId val="85042304"/>
-        <c:axId val="85043840"/>
+        <c:axId val="86446080"/>
+        <c:axId val="86447616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="85042304"/>
+        <c:axId val="86446080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2194,14 +2192,14 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85043840"/>
+        <c:crossAx val="86447616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85043840"/>
+        <c:axId val="86447616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2250,7 +2248,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85042304"/>
+        <c:crossAx val="86446080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2292,7 +2290,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2333,7 +2331,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2479,13 +2476,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:marker val="1"/>
-        <c:axId val="84363520"/>
-        <c:axId val="84373504"/>
+        <c:axId val="86475904"/>
+        <c:axId val="86477440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84363520"/>
+        <c:axId val="86475904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2525,14 +2521,14 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84373504"/>
+        <c:crossAx val="86477440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84373504"/>
+        <c:axId val="86477440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2581,7 +2577,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84363520"/>
+        <c:crossAx val="86475904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2623,7 +2619,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2659,7 +2655,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2805,13 +2800,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:marker val="1"/>
-        <c:axId val="88141824"/>
-        <c:axId val="88143360"/>
+        <c:axId val="86575744"/>
+        <c:axId val="86577536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="88141824"/>
+        <c:axId val="86575744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2851,14 +2845,14 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88143360"/>
+        <c:crossAx val="86577536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88143360"/>
+        <c:axId val="86577536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2907,7 +2901,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88141824"/>
+        <c:crossAx val="86575744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2949,7 +2943,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2985,7 +2979,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -3131,13 +3124,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:marker val="1"/>
-        <c:axId val="88044672"/>
-        <c:axId val="88046208"/>
+        <c:axId val="86618112"/>
+        <c:axId val="86619648"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="88044672"/>
+        <c:axId val="86618112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3177,14 +3169,14 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88046208"/>
+        <c:crossAx val="86619648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88046208"/>
+        <c:axId val="86619648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3233,7 +3225,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88044672"/>
+        <c:crossAx val="86618112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3275,7 +3267,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3399,24 +3391,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="83195392"/>
-        <c:axId val="83196928"/>
+        <c:axId val="86634496"/>
+        <c:axId val="86636032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="83195392"/>
+        <c:axId val="86634496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83196928"/>
+        <c:crossAx val="86636032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83196928"/>
+        <c:axId val="86636032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3424,7 +3416,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.000000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83195392"/>
+        <c:crossAx val="86634496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3433,7 +3425,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3557,24 +3549,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="93477888"/>
-        <c:axId val="87483136"/>
+        <c:axId val="109310336"/>
+        <c:axId val="109311872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="93477888"/>
+        <c:axId val="109310336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87483136"/>
+        <c:crossAx val="109311872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87483136"/>
+        <c:axId val="109311872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3582,7 +3574,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.000000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93477888"/>
+        <c:crossAx val="109310336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3591,7 +3583,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3858,31 +3850,31 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="reducido1_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="reducido2_1" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="reducido2" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="reducido3_1" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="reducido3" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="reducido1_2" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="reducido1_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="reducido2_1" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="reducido2" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ResumenP30G30" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ResumenP30G30" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="reducido1_2" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4140,7 +4132,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4163,141 +4155,159 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="B1" s="132" t="s">
+      <c r="B1" s="124" t="s">
         <v>309</v>
       </c>
-      <c r="C1" s="132"/>
-      <c r="D1" s="133" t="s">
+      <c r="C1" s="124"/>
+      <c r="D1" s="125" t="s">
         <v>310</v>
       </c>
-      <c r="E1" s="133"/>
+      <c r="E1" s="125"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="131" t="s">
+      <c r="A2" s="123" t="s">
         <v>311</v>
       </c>
-      <c r="B2" s="134">
+      <c r="B2" s="126">
         <v>0.7417797604166666</v>
       </c>
-      <c r="C2" s="134"/>
-      <c r="D2" s="113">
+      <c r="C2" s="126"/>
+      <c r="D2" s="127">
         <v>82.624184187499978</v>
       </c>
-      <c r="E2" s="113"/>
+      <c r="E2" s="127"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="131" t="s">
+      <c r="A3" s="123" t="s">
         <v>312</v>
       </c>
-      <c r="B3" s="134">
+      <c r="B3" s="126">
         <v>0.76057713541666661</v>
       </c>
-      <c r="C3" s="134"/>
-      <c r="D3" s="113">
+      <c r="C3" s="126"/>
+      <c r="D3" s="127">
         <v>122.69031959375</v>
       </c>
-      <c r="E3" s="113"/>
+      <c r="E3" s="127"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="131" t="s">
+      <c r="A4" s="123" t="s">
         <v>313</v>
       </c>
-      <c r="B4" s="134">
+      <c r="B4" s="126">
         <v>0.77727822916666667</v>
       </c>
-      <c r="C4" s="134"/>
-      <c r="D4" s="113">
+      <c r="C4" s="126"/>
+      <c r="D4" s="127">
         <v>266.41320669791668</v>
       </c>
-      <c r="E4" s="113"/>
+      <c r="E4" s="127"/>
     </row>
     <row r="6" spans="1:7" ht="15" thickBot="1"/>
     <row r="7" spans="1:7">
-      <c r="B7" s="143" t="s">
+      <c r="B7" s="141" t="s">
         <v>311</v>
       </c>
-      <c r="C7" s="144"/>
-      <c r="D7" s="150" t="s">
+      <c r="C7" s="152"/>
+      <c r="D7" s="138" t="s">
         <v>312</v>
       </c>
-      <c r="E7" s="151"/>
-      <c r="F7" s="149" t="s">
+      <c r="E7" s="139"/>
+      <c r="F7" s="140" t="s">
         <v>313</v>
       </c>
-      <c r="G7" s="143"/>
+      <c r="G7" s="141"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="B8" s="135" t="s">
+      <c r="B8" s="148" t="s">
         <v>284</v>
       </c>
-      <c r="C8" s="145"/>
-      <c r="D8" s="152" t="s">
+      <c r="C8" s="130"/>
+      <c r="D8" s="142" t="s">
         <v>284</v>
       </c>
-      <c r="E8" s="153"/>
-      <c r="F8" s="145" t="s">
+      <c r="E8" s="143"/>
+      <c r="F8" s="130" t="s">
         <v>284</v>
       </c>
-      <c r="G8" s="136"/>
+      <c r="G8" s="131"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="B9" s="137" t="s">
+      <c r="B9" s="149" t="s">
         <v>290</v>
       </c>
-      <c r="C9" s="146"/>
-      <c r="D9" s="154" t="s">
+      <c r="C9" s="132"/>
+      <c r="D9" s="144" t="s">
         <v>304</v>
       </c>
-      <c r="E9" s="155"/>
-      <c r="F9" s="146" t="s">
+      <c r="E9" s="145"/>
+      <c r="F9" s="132" t="s">
         <v>290</v>
       </c>
-      <c r="G9" s="138"/>
+      <c r="G9" s="133"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="B10" s="139" t="s">
+      <c r="B10" s="150" t="s">
         <v>295</v>
       </c>
-      <c r="C10" s="147"/>
-      <c r="D10" s="154" t="s">
+      <c r="C10" s="134"/>
+      <c r="D10" s="144" t="s">
         <v>295</v>
       </c>
-      <c r="E10" s="155"/>
-      <c r="F10" s="147" t="s">
+      <c r="E10" s="145"/>
+      <c r="F10" s="134" t="s">
         <v>295</v>
       </c>
-      <c r="G10" s="140"/>
+      <c r="G10" s="135"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="B11" s="137" t="s">
+      <c r="B11" s="149" t="s">
         <v>301</v>
       </c>
-      <c r="C11" s="146"/>
-      <c r="D11" s="156" t="s">
+      <c r="C11" s="132"/>
+      <c r="D11" s="146" t="s">
         <v>301</v>
       </c>
-      <c r="E11" s="157"/>
-      <c r="F11" s="146" t="s">
+      <c r="E11" s="147"/>
+      <c r="F11" s="132" t="s">
         <v>308</v>
       </c>
-      <c r="G11" s="138"/>
+      <c r="G11" s="133"/>
     </row>
     <row r="12" spans="1:7" ht="15" thickBot="1">
-      <c r="B12" s="141" t="s">
+      <c r="B12" s="151" t="s">
         <v>302</v>
       </c>
-      <c r="C12" s="148"/>
-      <c r="D12" s="158" t="s">
+      <c r="C12" s="136"/>
+      <c r="D12" s="128" t="s">
         <v>305</v>
       </c>
-      <c r="E12" s="159"/>
-      <c r="F12" s="148" t="s">
+      <c r="E12" s="129"/>
+      <c r="F12" s="136" t="s">
         <v>305</v>
       </c>
-      <c r="G12" s="142"/>
+      <c r="G12" s="137"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="D11:E11"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="B2:C2"/>
@@ -4306,24 +4316,6 @@
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B7:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4346,16 +4338,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="B1" s="114" t="s">
+      <c r="B1" s="153" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
+      <c r="C1" s="153"/>
+      <c r="D1" s="153"/>
+      <c r="E1" s="153"/>
+      <c r="F1" s="153"/>
+      <c r="G1" s="153"/>
+      <c r="H1" s="153"/>
+      <c r="I1" s="153"/>
       <c r="K1" t="s">
         <v>276</v>
       </c>
@@ -4370,18 +4362,18 @@
       </c>
     </row>
     <row r="2" spans="1:15">
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="154" t="s">
         <v>282</v>
       </c>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="115" t="s">
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="155" t="s">
         <v>281</v>
       </c>
-      <c r="G2" s="115"/>
-      <c r="H2" s="115"/>
-      <c r="I2" s="115"/>
+      <c r="G2" s="155"/>
+      <c r="H2" s="155"/>
+      <c r="I2" s="155"/>
       <c r="K2" t="s">
         <v>276</v>
       </c>
@@ -6002,20 +5994,20 @@
       </c>
     </row>
     <row r="36" spans="1:15">
-      <c r="C36" s="127" t="s">
+      <c r="C36" s="156" t="s">
         <v>309</v>
       </c>
-      <c r="D36" s="127"/>
-      <c r="E36" s="126">
+      <c r="D36" s="156"/>
+      <c r="E36" s="120">
         <f>AVERAGE(E4:E35)</f>
         <v>0.7417797604166666</v>
       </c>
-      <c r="F36" s="128"/>
-      <c r="G36" s="129" t="s">
+      <c r="F36" s="121"/>
+      <c r="G36" s="157" t="s">
         <v>310</v>
       </c>
-      <c r="H36" s="129"/>
-      <c r="I36" s="130">
+      <c r="H36" s="157"/>
+      <c r="I36" s="122">
         <f>AVERAGE(I4:I35)</f>
         <v>82.624184187499978</v>
       </c>
@@ -6047,10 +6039,10 @@
       </c>
     </row>
     <row r="38" spans="1:15">
-      <c r="A38" s="112" t="s">
+      <c r="A38" s="154" t="s">
         <v>279</v>
       </c>
-      <c r="B38" s="112"/>
+      <c r="B38" s="154"/>
       <c r="C38" s="37">
         <f>AVERAGE(E4:E19)</f>
         <v>0.73791177083333337</v>
@@ -6059,14 +6051,14 @@
         <f>AVERAGE(I4:I19)</f>
         <v>68.9744659375</v>
       </c>
-      <c r="E38" s="113" t="s">
+      <c r="E38" s="127" t="s">
         <v>280</v>
       </c>
-      <c r="F38" s="113"/>
-      <c r="H38" s="111" t="s">
+      <c r="F38" s="127"/>
+      <c r="H38" s="158" t="s">
         <v>284</v>
       </c>
-      <c r="I38" s="111"/>
+      <c r="I38" s="158"/>
       <c r="K38" t="s">
         <v>276</v>
       </c>
@@ -6081,10 +6073,10 @@
       </c>
     </row>
     <row r="39" spans="1:15">
-      <c r="A39" s="112" t="s">
+      <c r="A39" s="154" t="s">
         <v>278</v>
       </c>
-      <c r="B39" s="112"/>
+      <c r="B39" s="154"/>
       <c r="C39" s="37">
         <f>AVERAGE(E20:E35)</f>
         <v>0.74564775000000005</v>
@@ -6093,10 +6085,10 @@
         <f>AVERAGE(I20:I35)</f>
         <v>96.273902437499999</v>
       </c>
-      <c r="E39" s="113" t="s">
+      <c r="E39" s="127" t="s">
         <v>288</v>
       </c>
-      <c r="F39" s="113"/>
+      <c r="F39" s="127"/>
       <c r="K39" t="s">
         <v>276</v>
       </c>
@@ -6150,10 +6142,10 @@
       </c>
     </row>
     <row r="42" spans="1:15">
-      <c r="A42" s="112" t="s">
+      <c r="A42" s="154" t="s">
         <v>285</v>
       </c>
-      <c r="B42" s="112"/>
+      <c r="B42" s="154"/>
       <c r="C42" s="37">
         <f>AVERAGE(E4:E11)</f>
         <v>0.74170825000000007</v>
@@ -6162,14 +6154,14 @@
         <f>AVERAGE(I4:I11)</f>
         <v>73.842973583333332</v>
       </c>
-      <c r="E42" s="113" t="s">
+      <c r="E42" s="127" t="s">
         <v>287</v>
       </c>
-      <c r="F42" s="113"/>
-      <c r="H42" s="110" t="s">
+      <c r="F42" s="127"/>
+      <c r="H42" s="159" t="s">
         <v>290</v>
       </c>
-      <c r="I42" s="110"/>
+      <c r="I42" s="159"/>
       <c r="K42" t="s">
         <v>276</v>
       </c>
@@ -6184,10 +6176,10 @@
       </c>
     </row>
     <row r="43" spans="1:15">
-      <c r="A43" s="112" t="s">
+      <c r="A43" s="154" t="s">
         <v>286</v>
       </c>
-      <c r="B43" s="112"/>
+      <c r="B43" s="154"/>
       <c r="C43" s="37">
         <f>AVERAGE(E12:E19)</f>
         <v>0.73411529166666667</v>
@@ -6196,10 +6188,10 @@
         <f>AVERAGE(I12:I19)</f>
         <v>64.105958291666667</v>
       </c>
-      <c r="E43" s="113" t="s">
+      <c r="E43" s="127" t="s">
         <v>289</v>
       </c>
-      <c r="F43" s="113"/>
+      <c r="F43" s="127"/>
       <c r="K43" t="s">
         <v>276</v>
       </c>
@@ -6253,10 +6245,10 @@
       </c>
     </row>
     <row r="46" spans="1:15">
-      <c r="A46" s="112" t="s">
+      <c r="A46" s="154" t="s">
         <v>291</v>
       </c>
-      <c r="B46" s="112"/>
+      <c r="B46" s="154"/>
       <c r="C46" s="37">
         <f>AVERAGE(E12:E15)</f>
         <v>0.72639283333333338</v>
@@ -6265,14 +6257,14 @@
         <f>AVERAGE(I12:I15)</f>
         <v>52.946694916666672</v>
       </c>
-      <c r="E46" s="113" t="s">
+      <c r="E46" s="127" t="s">
         <v>293</v>
       </c>
-      <c r="F46" s="113"/>
-      <c r="H46" s="111" t="s">
+      <c r="F46" s="127"/>
+      <c r="H46" s="158" t="s">
         <v>295</v>
       </c>
-      <c r="I46" s="111"/>
+      <c r="I46" s="158"/>
       <c r="K46" t="s">
         <v>276</v>
       </c>
@@ -6287,10 +6279,10 @@
       </c>
     </row>
     <row r="47" spans="1:15">
-      <c r="A47" s="112" t="s">
+      <c r="A47" s="154" t="s">
         <v>292</v>
       </c>
-      <c r="B47" s="112"/>
+      <c r="B47" s="154"/>
       <c r="C47" s="37">
         <f>AVERAGE(E16:E19)</f>
         <v>0.74183775000000007</v>
@@ -6299,10 +6291,10 @@
         <f>AVERAGE(I16:I19)</f>
         <v>75.265221666666662</v>
       </c>
-      <c r="E47" s="113" t="s">
+      <c r="E47" s="127" t="s">
         <v>294</v>
       </c>
-      <c r="F47" s="113"/>
+      <c r="F47" s="127"/>
       <c r="K47" t="s">
         <v>276</v>
       </c>
@@ -6551,10 +6543,10 @@
       </c>
     </row>
     <row r="56" spans="1:15">
-      <c r="A56" s="112" t="s">
+      <c r="A56" s="154" t="s">
         <v>297</v>
       </c>
-      <c r="B56" s="112"/>
+      <c r="B56" s="154"/>
       <c r="C56" s="37">
         <f>AVERAGE(E51:E52)</f>
         <v>0.72057600000000011</v>
@@ -6563,14 +6555,14 @@
         <f>AVERAGE(I51:I52)</f>
         <v>47.367375666666668</v>
       </c>
-      <c r="E56" s="113" t="s">
+      <c r="E56" s="127" t="s">
         <v>299</v>
       </c>
-      <c r="F56" s="113"/>
-      <c r="H56" s="110" t="s">
+      <c r="F56" s="127"/>
+      <c r="H56" s="159" t="s">
         <v>301</v>
       </c>
-      <c r="I56" s="110"/>
+      <c r="I56" s="159"/>
       <c r="K56" t="s">
         <v>276</v>
       </c>
@@ -6585,10 +6577,10 @@
       </c>
     </row>
     <row r="57" spans="1:15">
-      <c r="A57" s="112" t="s">
+      <c r="A57" s="154" t="s">
         <v>298</v>
       </c>
-      <c r="B57" s="112"/>
+      <c r="B57" s="154"/>
       <c r="C57" s="37">
         <f>AVERAGE(E53:E54)</f>
         <v>0.73220966666666665</v>
@@ -6597,10 +6589,10 @@
         <f>AVERAGE(I53:I54)</f>
         <v>58.526014166666663</v>
       </c>
-      <c r="E57" s="113" t="s">
+      <c r="E57" s="127" t="s">
         <v>300</v>
       </c>
-      <c r="F57" s="113"/>
+      <c r="F57" s="127"/>
       <c r="K57" t="s">
         <v>276</v>
       </c>
@@ -6640,10 +6632,10 @@
       </c>
     </row>
     <row r="59" spans="1:15">
-      <c r="H59" s="110" t="s">
+      <c r="H59" s="159" t="s">
         <v>302</v>
       </c>
-      <c r="I59" s="110"/>
+      <c r="I59" s="159"/>
       <c r="K59" t="s">
         <v>276</v>
       </c>
@@ -6686,10 +6678,10 @@
       </c>
     </row>
     <row r="62" spans="1:15">
-      <c r="A62" s="111" t="s">
+      <c r="A62" s="158" t="s">
         <v>284</v>
       </c>
-      <c r="B62" s="111"/>
+      <c r="B62" s="158"/>
       <c r="K62" t="s">
         <v>276</v>
       </c>
@@ -6704,10 +6696,10 @@
       </c>
     </row>
     <row r="63" spans="1:15">
-      <c r="A63" s="110" t="s">
+      <c r="A63" s="159" t="s">
         <v>290</v>
       </c>
-      <c r="B63" s="110"/>
+      <c r="B63" s="159"/>
       <c r="K63" t="s">
         <v>276</v>
       </c>
@@ -6722,10 +6714,10 @@
       </c>
     </row>
     <row r="64" spans="1:15">
-      <c r="A64" s="111" t="s">
+      <c r="A64" s="158" t="s">
         <v>295</v>
       </c>
-      <c r="B64" s="111"/>
+      <c r="B64" s="158"/>
       <c r="K64" t="s">
         <v>276</v>
       </c>
@@ -6740,10 +6732,10 @@
       </c>
     </row>
     <row r="65" spans="1:15">
-      <c r="A65" s="110" t="s">
+      <c r="A65" s="159" t="s">
         <v>301</v>
       </c>
-      <c r="B65" s="110"/>
+      <c r="B65" s="159"/>
       <c r="K65" t="s">
         <v>276</v>
       </c>
@@ -6758,10 +6750,10 @@
       </c>
     </row>
     <row r="66" spans="1:15">
-      <c r="A66" s="110" t="s">
+      <c r="A66" s="159" t="s">
         <v>302</v>
       </c>
-      <c r="B66" s="110"/>
+      <c r="B66" s="159"/>
       <c r="K66" t="s">
         <v>276</v>
       </c>
@@ -7224,13 +7216,22 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="H46:I46"/>
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="E39:F39"/>
     <mergeCell ref="H38:I38"/>
@@ -7239,22 +7240,13 @@
     <mergeCell ref="E42:F42"/>
     <mergeCell ref="E43:F43"/>
     <mergeCell ref="H42:I42"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="G36:H36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7276,16 +7268,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="B1" s="114" t="s">
+      <c r="B1" s="153" t="s">
         <v>303</v>
       </c>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
+      <c r="C1" s="153"/>
+      <c r="D1" s="153"/>
+      <c r="E1" s="153"/>
+      <c r="F1" s="153"/>
+      <c r="G1" s="153"/>
+      <c r="H1" s="153"/>
+      <c r="I1" s="153"/>
       <c r="K1" t="s">
         <v>276</v>
       </c>
@@ -7300,18 +7292,18 @@
       </c>
     </row>
     <row r="2" spans="1:15">
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="154" t="s">
         <v>282</v>
       </c>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="115" t="s">
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="155" t="s">
         <v>281</v>
       </c>
-      <c r="G2" s="115"/>
-      <c r="H2" s="115"/>
-      <c r="I2" s="115"/>
+      <c r="G2" s="155"/>
+      <c r="H2" s="155"/>
+      <c r="I2" s="155"/>
       <c r="K2" t="s">
         <v>276</v>
       </c>
@@ -8932,20 +8924,20 @@
       </c>
     </row>
     <row r="36" spans="1:15">
-      <c r="C36" s="127" t="s">
+      <c r="C36" s="156" t="s">
         <v>309</v>
       </c>
-      <c r="D36" s="127"/>
-      <c r="E36" s="126">
+      <c r="D36" s="156"/>
+      <c r="E36" s="120">
         <f>AVERAGE(E4:E35)</f>
         <v>0.76057713541666661</v>
       </c>
-      <c r="F36" s="128"/>
-      <c r="G36" s="129" t="s">
+      <c r="F36" s="121"/>
+      <c r="G36" s="157" t="s">
         <v>310</v>
       </c>
-      <c r="H36" s="129"/>
-      <c r="I36" s="130">
+      <c r="H36" s="157"/>
+      <c r="I36" s="122">
         <f>AVERAGE(I4:I35)</f>
         <v>122.69031959375</v>
       </c>
@@ -8977,10 +8969,10 @@
       </c>
     </row>
     <row r="38" spans="1:15">
-      <c r="A38" s="112" t="s">
+      <c r="A38" s="154" t="s">
         <v>279</v>
       </c>
-      <c r="B38" s="112"/>
+      <c r="B38" s="154"/>
       <c r="C38" s="37">
         <f>AVERAGE(E4:E19)</f>
         <v>0.75820720833333333</v>
@@ -8989,14 +8981,14 @@
         <f>AVERAGE(I4:I19)</f>
         <v>101.81007320833332</v>
       </c>
-      <c r="E38" s="113" t="s">
+      <c r="E38" s="127" t="s">
         <v>280</v>
       </c>
-      <c r="F38" s="113"/>
-      <c r="H38" s="111" t="s">
+      <c r="F38" s="127"/>
+      <c r="H38" s="158" t="s">
         <v>284</v>
       </c>
-      <c r="I38" s="111"/>
+      <c r="I38" s="158"/>
       <c r="K38" t="s">
         <v>276</v>
       </c>
@@ -9011,10 +9003,10 @@
       </c>
     </row>
     <row r="39" spans="1:15">
-      <c r="A39" s="112" t="s">
+      <c r="A39" s="154" t="s">
         <v>278</v>
       </c>
-      <c r="B39" s="112"/>
+      <c r="B39" s="154"/>
       <c r="C39" s="37">
         <f>AVERAGE(E20:E35)</f>
         <v>0.7629470625</v>
@@ -9023,10 +9015,10 @@
         <f>AVERAGE(I20:I35)</f>
         <v>143.57056597916667</v>
       </c>
-      <c r="E39" s="113" t="s">
+      <c r="E39" s="127" t="s">
         <v>288</v>
       </c>
-      <c r="F39" s="113"/>
+      <c r="F39" s="127"/>
       <c r="K39" t="s">
         <v>276</v>
       </c>
@@ -9080,10 +9072,10 @@
       </c>
     </row>
     <row r="42" spans="1:15">
-      <c r="A42" s="112" t="s">
+      <c r="A42" s="154" t="s">
         <v>285</v>
       </c>
-      <c r="B42" s="112"/>
+      <c r="B42" s="154"/>
       <c r="C42" s="37">
         <f>AVERAGE(E4:E11)</f>
         <v>0.75591520833333326</v>
@@ -9092,14 +9084,14 @@
         <f>AVERAGE(I4:I11)</f>
         <v>99.442729416666666</v>
       </c>
-      <c r="E42" s="113" t="s">
+      <c r="E42" s="127" t="s">
         <v>287</v>
       </c>
-      <c r="F42" s="113"/>
-      <c r="H42" s="111" t="s">
+      <c r="F42" s="127"/>
+      <c r="H42" s="158" t="s">
         <v>304</v>
       </c>
-      <c r="I42" s="111"/>
+      <c r="I42" s="158"/>
       <c r="K42" t="s">
         <v>276</v>
       </c>
@@ -9114,10 +9106,10 @@
       </c>
     </row>
     <row r="43" spans="1:15">
-      <c r="A43" s="112" t="s">
+      <c r="A43" s="154" t="s">
         <v>286</v>
       </c>
-      <c r="B43" s="112"/>
+      <c r="B43" s="154"/>
       <c r="C43" s="37">
         <f>AVERAGE(E12:E19)</f>
         <v>0.7604992083333334</v>
@@ -9126,10 +9118,10 @@
         <f>AVERAGE(I12:I19)</f>
         <v>104.17741700000001</v>
       </c>
-      <c r="E43" s="113" t="s">
+      <c r="E43" s="127" t="s">
         <v>289</v>
       </c>
-      <c r="F43" s="113"/>
+      <c r="F43" s="127"/>
       <c r="K43" t="s">
         <v>276</v>
       </c>
@@ -9183,10 +9175,10 @@
       </c>
     </row>
     <row r="46" spans="1:15">
-      <c r="A46" s="112" t="s">
+      <c r="A46" s="154" t="s">
         <v>291</v>
       </c>
-      <c r="B46" s="112"/>
+      <c r="B46" s="154"/>
       <c r="C46" s="37">
         <f>AVERAGE(E4:E7)</f>
         <v>0.73975449999999998</v>
@@ -9195,14 +9187,14 @@
         <f>AVERAGE(I4:I7)</f>
         <v>80.383680916666663</v>
       </c>
-      <c r="E46" s="113" t="s">
+      <c r="E46" s="127" t="s">
         <v>293</v>
       </c>
-      <c r="F46" s="113"/>
-      <c r="H46" s="111" t="s">
+      <c r="F46" s="127"/>
+      <c r="H46" s="158" t="s">
         <v>295</v>
       </c>
-      <c r="I46" s="111"/>
+      <c r="I46" s="158"/>
       <c r="K46" t="s">
         <v>276</v>
       </c>
@@ -9217,10 +9209,10 @@
       </c>
     </row>
     <row r="47" spans="1:15">
-      <c r="A47" s="112" t="s">
+      <c r="A47" s="154" t="s">
         <v>292</v>
       </c>
-      <c r="B47" s="112"/>
+      <c r="B47" s="154"/>
       <c r="C47" s="37">
         <f>AVERAGE(E8:E11)</f>
         <v>0.77207591666666664</v>
@@ -9229,10 +9221,10 @@
         <f>AVERAGE(I8:I11)</f>
         <v>118.50177791666667</v>
       </c>
-      <c r="E47" s="113" t="s">
+      <c r="E47" s="127" t="s">
         <v>294</v>
       </c>
-      <c r="F47" s="113"/>
+      <c r="F47" s="127"/>
       <c r="K47" t="s">
         <v>276</v>
       </c>
@@ -9481,10 +9473,10 @@
       </c>
     </row>
     <row r="56" spans="1:15">
-      <c r="A56" s="112" t="s">
+      <c r="A56" s="154" t="s">
         <v>297</v>
       </c>
-      <c r="B56" s="112"/>
+      <c r="B56" s="154"/>
       <c r="C56" s="37">
         <f>AVERAGE(E51:E52)</f>
         <v>0.73917716666666666</v>
@@ -9493,14 +9485,14 @@
         <f>AVERAGE(I51:I52)</f>
         <v>78.314479166666672</v>
       </c>
-      <c r="E56" s="113" t="s">
+      <c r="E56" s="127" t="s">
         <v>299</v>
       </c>
-      <c r="F56" s="113"/>
-      <c r="H56" s="110" t="s">
+      <c r="F56" s="127"/>
+      <c r="H56" s="159" t="s">
         <v>301</v>
       </c>
-      <c r="I56" s="110"/>
+      <c r="I56" s="159"/>
       <c r="K56" t="s">
         <v>276</v>
       </c>
@@ -9515,10 +9507,10 @@
       </c>
     </row>
     <row r="57" spans="1:15">
-      <c r="A57" s="112" t="s">
+      <c r="A57" s="154" t="s">
         <v>298</v>
       </c>
-      <c r="B57" s="112"/>
+      <c r="B57" s="154"/>
       <c r="C57" s="37">
         <f>AVERAGE(E53:E54)</f>
         <v>0.7403318333333333</v>
@@ -9527,10 +9519,10 @@
         <f>AVERAGE(I53:I54)</f>
         <v>82.452882666666653</v>
       </c>
-      <c r="E57" s="113" t="s">
+      <c r="E57" s="127" t="s">
         <v>300</v>
       </c>
-      <c r="F57" s="113"/>
+      <c r="F57" s="127"/>
       <c r="K57" t="s">
         <v>276</v>
       </c>
@@ -9570,11 +9562,11 @@
       </c>
     </row>
     <row r="59" spans="1:15">
-      <c r="D59" s="125"/>
-      <c r="H59" s="110" t="s">
+      <c r="D59" s="119"/>
+      <c r="H59" s="159" t="s">
         <v>305</v>
       </c>
-      <c r="I59" s="110"/>
+      <c r="I59" s="159"/>
       <c r="K59" t="s">
         <v>276</v>
       </c>
@@ -9617,10 +9609,10 @@
       </c>
     </row>
     <row r="62" spans="1:15">
-      <c r="A62" s="111" t="s">
+      <c r="A62" s="158" t="s">
         <v>284</v>
       </c>
-      <c r="B62" s="111"/>
+      <c r="B62" s="158"/>
       <c r="K62" t="s">
         <v>276</v>
       </c>
@@ -9635,10 +9627,10 @@
       </c>
     </row>
     <row r="63" spans="1:15">
-      <c r="A63" s="111" t="s">
+      <c r="A63" s="158" t="s">
         <v>304</v>
       </c>
-      <c r="B63" s="111"/>
+      <c r="B63" s="158"/>
       <c r="K63" t="s">
         <v>276</v>
       </c>
@@ -9653,10 +9645,10 @@
       </c>
     </row>
     <row r="64" spans="1:15">
-      <c r="A64" s="111" t="s">
+      <c r="A64" s="158" t="s">
         <v>295</v>
       </c>
-      <c r="B64" s="111"/>
+      <c r="B64" s="158"/>
       <c r="K64" t="s">
         <v>276</v>
       </c>
@@ -9671,10 +9663,10 @@
       </c>
     </row>
     <row r="65" spans="1:15">
-      <c r="A65" s="110" t="s">
+      <c r="A65" s="159" t="s">
         <v>301</v>
       </c>
-      <c r="B65" s="110"/>
+      <c r="B65" s="159"/>
       <c r="K65" t="s">
         <v>276</v>
       </c>
@@ -9689,10 +9681,10 @@
       </c>
     </row>
     <row r="66" spans="1:15">
-      <c r="A66" s="110" t="s">
+      <c r="A66" s="159" t="s">
         <v>305</v>
       </c>
-      <c r="B66" s="110"/>
+      <c r="B66" s="159"/>
       <c r="K66" t="s">
         <v>276</v>
       </c>
@@ -10155,14 +10147,14 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
     <mergeCell ref="A56:B56"/>
     <mergeCell ref="E56:F56"/>
     <mergeCell ref="H56:I56"/>
@@ -10178,14 +10170,14 @@
     <mergeCell ref="H46:I46"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="E47:F47"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="G36:H36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -10207,16 +10199,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="B1" s="114" t="s">
+      <c r="B1" s="153" t="s">
         <v>306</v>
       </c>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
+      <c r="C1" s="153"/>
+      <c r="D1" s="153"/>
+      <c r="E1" s="153"/>
+      <c r="F1" s="153"/>
+      <c r="G1" s="153"/>
+      <c r="H1" s="153"/>
+      <c r="I1" s="153"/>
       <c r="K1" t="s">
         <v>276</v>
       </c>
@@ -10231,18 +10223,18 @@
       </c>
     </row>
     <row r="2" spans="1:15">
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="154" t="s">
         <v>282</v>
       </c>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="115" t="s">
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="155" t="s">
         <v>281</v>
       </c>
-      <c r="G2" s="115"/>
-      <c r="H2" s="115"/>
-      <c r="I2" s="115"/>
+      <c r="G2" s="155"/>
+      <c r="H2" s="155"/>
+      <c r="I2" s="155"/>
       <c r="K2" t="s">
         <v>276</v>
       </c>
@@ -10326,7 +10318,7 @@
         <f>O3</f>
         <v>84.396827000000002</v>
       </c>
-      <c r="I4" s="116">
+      <c r="I4" s="110">
         <f t="shared" ref="I4:I35" si="1">AVERAGE(F4:H4)</f>
         <v>115.16425366666665</v>
       </c>
@@ -10785,18 +10777,18 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="15" thickBot="1">
-      <c r="A14" s="117" t="s">
+      <c r="A14" s="111" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="118">
+      <c r="B14" s="112">
         <f>L31</f>
         <v>0.77724599999999999</v>
       </c>
-      <c r="C14" s="119">
+      <c r="C14" s="113">
         <f>L32</f>
         <v>0.85101599999999999</v>
       </c>
-      <c r="D14" s="120">
+      <c r="D14" s="114">
         <f>L33</f>
         <v>0.76990599999999998</v>
       </c>
@@ -10804,15 +10796,15 @@
         <f t="shared" si="0"/>
         <v>0.7993893333333334</v>
       </c>
-      <c r="F14" s="121">
+      <c r="F14" s="115">
         <f>O31</f>
         <v>276.67182500000001</v>
       </c>
-      <c r="G14" s="122">
+      <c r="G14" s="116">
         <f>O32</f>
         <v>101.38579900000001</v>
       </c>
-      <c r="H14" s="123">
+      <c r="H14" s="117">
         <f>O33</f>
         <v>230.21716799999999</v>
       </c>
@@ -10865,7 +10857,7 @@
         <f>O36</f>
         <v>306.48953</v>
       </c>
-      <c r="I15" s="124">
+      <c r="I15" s="118">
         <f t="shared" si="1"/>
         <v>238.73632166666667</v>
       </c>
@@ -11863,20 +11855,20 @@
       </c>
     </row>
     <row r="36" spans="1:15">
-      <c r="C36" s="127" t="s">
+      <c r="C36" s="156" t="s">
         <v>309</v>
       </c>
-      <c r="D36" s="127"/>
-      <c r="E36" s="126">
+      <c r="D36" s="156"/>
+      <c r="E36" s="120">
         <f>AVERAGE(E4:E35)</f>
         <v>0.77727822916666667</v>
       </c>
-      <c r="F36" s="128"/>
-      <c r="G36" s="129" t="s">
+      <c r="F36" s="121"/>
+      <c r="G36" s="157" t="s">
         <v>310</v>
       </c>
-      <c r="H36" s="129"/>
-      <c r="I36" s="130">
+      <c r="H36" s="157"/>
+      <c r="I36" s="122">
         <f>AVERAGE(I4:I35)</f>
         <v>266.41320669791668</v>
       </c>
@@ -11908,10 +11900,10 @@
       </c>
     </row>
     <row r="38" spans="1:15">
-      <c r="A38" s="112" t="s">
+      <c r="A38" s="154" t="s">
         <v>279</v>
       </c>
-      <c r="B38" s="112"/>
+      <c r="B38" s="154"/>
       <c r="C38" s="37">
         <f>AVERAGE(E4:E19)</f>
         <v>0.77869508333333337</v>
@@ -11920,14 +11912,14 @@
         <f>AVERAGE(I4:I19)</f>
         <v>239.27056056249998</v>
       </c>
-      <c r="E38" s="113" t="s">
+      <c r="E38" s="127" t="s">
         <v>280</v>
       </c>
-      <c r="F38" s="113"/>
-      <c r="H38" s="111" t="s">
+      <c r="F38" s="127"/>
+      <c r="H38" s="158" t="s">
         <v>284</v>
       </c>
-      <c r="I38" s="111"/>
+      <c r="I38" s="158"/>
       <c r="K38" t="s">
         <v>276</v>
       </c>
@@ -11942,10 +11934,10 @@
       </c>
     </row>
     <row r="39" spans="1:15">
-      <c r="A39" s="112" t="s">
+      <c r="A39" s="154" t="s">
         <v>278</v>
       </c>
-      <c r="B39" s="112"/>
+      <c r="B39" s="154"/>
       <c r="C39" s="37">
         <f>AVERAGE(E20:E35)</f>
         <v>0.77586137500000019</v>
@@ -11954,10 +11946,10 @@
         <f>AVERAGE(I20:I35)</f>
         <v>293.55585283333329</v>
       </c>
-      <c r="E39" s="113" t="s">
+      <c r="E39" s="127" t="s">
         <v>288</v>
       </c>
-      <c r="F39" s="113"/>
+      <c r="F39" s="127"/>
       <c r="K39" t="s">
         <v>276</v>
       </c>
@@ -12011,10 +12003,10 @@
       </c>
     </row>
     <row r="42" spans="1:15">
-      <c r="A42" s="112" t="s">
+      <c r="A42" s="154" t="s">
         <v>285</v>
       </c>
-      <c r="B42" s="112"/>
+      <c r="B42" s="154"/>
       <c r="C42" s="37">
         <f>AVERAGE(E4:E11)</f>
         <v>0.78718558333333322</v>
@@ -12023,14 +12015,14 @@
         <f>AVERAGE(I4:I11)</f>
         <v>246.04436458333333</v>
       </c>
-      <c r="E42" s="113" t="s">
+      <c r="E42" s="127" t="s">
         <v>287</v>
       </c>
-      <c r="F42" s="113"/>
-      <c r="H42" s="110" t="s">
+      <c r="F42" s="127"/>
+      <c r="H42" s="159" t="s">
         <v>290</v>
       </c>
-      <c r="I42" s="110"/>
+      <c r="I42" s="159"/>
       <c r="K42" t="s">
         <v>276</v>
       </c>
@@ -12045,10 +12037,10 @@
       </c>
     </row>
     <row r="43" spans="1:15">
-      <c r="A43" s="112" t="s">
+      <c r="A43" s="154" t="s">
         <v>286</v>
       </c>
-      <c r="B43" s="112"/>
+      <c r="B43" s="154"/>
       <c r="C43" s="37">
         <f>AVERAGE(E12:E19)</f>
         <v>0.77020458333333341</v>
@@ -12057,10 +12049,10 @@
         <f>AVERAGE(I12:I19)</f>
         <v>232.49675654166666</v>
       </c>
-      <c r="E43" s="113" t="s">
+      <c r="E43" s="127" t="s">
         <v>289</v>
       </c>
-      <c r="F43" s="113"/>
+      <c r="F43" s="127"/>
       <c r="K43" t="s">
         <v>276</v>
       </c>
@@ -12114,10 +12106,10 @@
       </c>
     </row>
     <row r="46" spans="1:15">
-      <c r="A46" s="112" t="s">
+      <c r="A46" s="154" t="s">
         <v>291</v>
       </c>
-      <c r="B46" s="112"/>
+      <c r="B46" s="154"/>
       <c r="C46" s="37">
         <f>AVERAGE(E12:E15)</f>
         <v>0.76954883333333335</v>
@@ -12126,14 +12118,14 @@
         <f>AVERAGE(I12:I15)</f>
         <v>183.06013725</v>
       </c>
-      <c r="E46" s="113" t="s">
+      <c r="E46" s="127" t="s">
         <v>293</v>
       </c>
-      <c r="F46" s="113"/>
-      <c r="H46" s="111" t="s">
+      <c r="F46" s="127"/>
+      <c r="H46" s="158" t="s">
         <v>295</v>
       </c>
-      <c r="I46" s="111"/>
+      <c r="I46" s="158"/>
       <c r="K46" t="s">
         <v>276</v>
       </c>
@@ -12148,10 +12140,10 @@
       </c>
     </row>
     <row r="47" spans="1:15">
-      <c r="A47" s="112" t="s">
+      <c r="A47" s="154" t="s">
         <v>292</v>
       </c>
-      <c r="B47" s="112"/>
+      <c r="B47" s="154"/>
       <c r="C47" s="37">
         <f>AVERAGE(E16:E19)</f>
         <v>0.77086033333333337</v>
@@ -12160,10 +12152,10 @@
         <f>AVERAGE(I16:I19)</f>
         <v>281.93337583333334</v>
       </c>
-      <c r="E47" s="113" t="s">
+      <c r="E47" s="127" t="s">
         <v>294</v>
       </c>
-      <c r="F47" s="113"/>
+      <c r="F47" s="127"/>
       <c r="K47" t="s">
         <v>276</v>
       </c>
@@ -12444,10 +12436,10 @@
       </c>
     </row>
     <row r="56" spans="1:15">
-      <c r="A56" s="112" t="s">
+      <c r="A56" s="154" t="s">
         <v>297</v>
       </c>
-      <c r="B56" s="112"/>
+      <c r="B56" s="154"/>
       <c r="C56" s="37">
         <f>AVERAGE(E51:E52)</f>
         <v>0.75453683333333343</v>
@@ -12456,14 +12448,14 @@
         <f>AVERAGE(I51:I52)</f>
         <v>310.25507883333336</v>
       </c>
-      <c r="E56" s="113" t="s">
+      <c r="E56" s="127" t="s">
         <v>299</v>
       </c>
-      <c r="F56" s="113"/>
-      <c r="H56" s="110" t="s">
+      <c r="F56" s="127"/>
+      <c r="H56" s="159" t="s">
         <v>308</v>
       </c>
-      <c r="I56" s="110"/>
+      <c r="I56" s="159"/>
       <c r="K56" t="s">
         <v>276</v>
       </c>
@@ -12478,10 +12470,10 @@
       </c>
     </row>
     <row r="57" spans="1:15">
-      <c r="A57" s="112" t="s">
+      <c r="A57" s="154" t="s">
         <v>298</v>
       </c>
-      <c r="B57" s="112"/>
+      <c r="B57" s="154"/>
       <c r="C57" s="37">
         <f>AVERAGE(E53:E54)</f>
         <v>0.73502549999999989</v>
@@ -12490,10 +12482,10 @@
         <f>AVERAGE(I53:I54)</f>
         <v>280.63521783333334</v>
       </c>
-      <c r="E57" s="113" t="s">
+      <c r="E57" s="127" t="s">
         <v>300</v>
       </c>
-      <c r="F57" s="113"/>
+      <c r="F57" s="127"/>
       <c r="K57" t="s">
         <v>276</v>
       </c>
@@ -12533,10 +12525,10 @@
       </c>
     </row>
     <row r="59" spans="1:15">
-      <c r="H59" s="110" t="s">
+      <c r="H59" s="159" t="s">
         <v>305</v>
       </c>
-      <c r="I59" s="110"/>
+      <c r="I59" s="159"/>
       <c r="K59" t="s">
         <v>276</v>
       </c>
@@ -12579,10 +12571,10 @@
       </c>
     </row>
     <row r="62" spans="1:15">
-      <c r="A62" s="111" t="s">
+      <c r="A62" s="158" t="s">
         <v>284</v>
       </c>
-      <c r="B62" s="111"/>
+      <c r="B62" s="158"/>
       <c r="K62" t="s">
         <v>276</v>
       </c>
@@ -12597,10 +12589,10 @@
       </c>
     </row>
     <row r="63" spans="1:15">
-      <c r="A63" s="110" t="s">
+      <c r="A63" s="159" t="s">
         <v>290</v>
       </c>
-      <c r="B63" s="110"/>
+      <c r="B63" s="159"/>
       <c r="K63" t="s">
         <v>276</v>
       </c>
@@ -12615,10 +12607,10 @@
       </c>
     </row>
     <row r="64" spans="1:15">
-      <c r="A64" s="111" t="s">
+      <c r="A64" s="158" t="s">
         <v>295</v>
       </c>
-      <c r="B64" s="111"/>
+      <c r="B64" s="158"/>
       <c r="K64" t="s">
         <v>276</v>
       </c>
@@ -12633,10 +12625,10 @@
       </c>
     </row>
     <row r="65" spans="1:15">
-      <c r="A65" s="110" t="s">
+      <c r="A65" s="159" t="s">
         <v>308</v>
       </c>
-      <c r="B65" s="110"/>
+      <c r="B65" s="159"/>
       <c r="K65" t="s">
         <v>276</v>
       </c>
@@ -12651,10 +12643,10 @@
       </c>
     </row>
     <row r="66" spans="1:15">
-      <c r="A66" s="110" t="s">
+      <c r="A66" s="159" t="s">
         <v>305</v>
       </c>
-      <c r="B66" s="110"/>
+      <c r="B66" s="159"/>
       <c r="K66" t="s">
         <v>276</v>
       </c>
@@ -13117,6 +13109,21 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="E43:F43"/>
     <mergeCell ref="A65:B65"/>
     <mergeCell ref="A66:B66"/>
     <mergeCell ref="C36:D36"/>
@@ -13133,21 +13140,6 @@
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="E47:F47"/>
     <mergeCell ref="A56:B56"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H38:I38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>